<commit_message>
shift priority indicated by asterisk
</commit_message>
<xml_diff>
--- a/schedule_template.xlsx
+++ b/schedule_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>SUN</t>
   </si>
@@ -70,25 +70,31 @@
     <t>14:30-17:30</t>
   </si>
   <si>
+    <t>2*</t>
+  </si>
+  <si>
+    <t>15:00-19:00</t>
+  </si>
+  <si>
+    <t>16:00-19:00</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>15:00-19:00</t>
-  </si>
-  <si>
-    <t>16:00-19:00</t>
-  </si>
-  <si>
     <t>19:00-23:00</t>
   </si>
   <si>
     <t>14:00-17:00</t>
   </si>
   <si>
+    <t>3*</t>
+  </si>
+  <si>
+    <t>17:00-21:00</t>
+  </si>
+  <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>17:00-21:00</t>
   </si>
 </sst>
 </file>
@@ -96,13 +102,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -138,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,8 +158,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,6 +172,9 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,19 +488,19 @@
     <col min="2" max="2" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +530,7 @@
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
@@ -541,7 +556,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -567,7 +582,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
@@ -595,7 +610,7 @@
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5" t="s">
@@ -623,7 +638,7 @@
       </c>
       <c r="N5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
@@ -647,7 +662,7 @@
       </c>
       <c r="N6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5" t="s">
@@ -671,7 +686,7 @@
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -697,9 +712,9 @@
       <c r="M8" s="3"/>
       <c r="N8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
@@ -723,13 +738,13 @@
       <c r="M9" s="3"/>
       <c r="N9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5" t="s">
@@ -745,15 +760,15 @@
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="3"/>
       <c r="N10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="5" t="s">
@@ -761,67 +776,67 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="3"/>
       <c r="N11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="3"/>
       <c r="N12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="3"/>

</xml_diff>

<commit_message>
gave up on individual position
</commit_message>
<xml_diff>
--- a/schedule_template.xlsx
+++ b/schedule_template.xlsx
@@ -102,7 +102,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,12 +113,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -158,7 +152,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -168,7 +162,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,7 +712,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5" t="s">
@@ -776,19 +770,19 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="3"/>

</xml_diff>

<commit_message>
minor bug fix, C now can read int with more than 1 digit
</commit_message>
<xml_diff>
--- a/schedule_template.xlsx
+++ b/schedule_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>SUN</t>
   </si>
@@ -46,6 +46,9 @@
     <t>1</t>
   </si>
   <si>
+    <t>1*</t>
+  </si>
+  <si>
     <t>10:30-14:30</t>
   </si>
   <si>
@@ -70,25 +73,16 @@
     <t>14:30-17:30</t>
   </si>
   <si>
-    <t>2*</t>
-  </si>
-  <si>
     <t>15:00-19:00</t>
   </si>
   <si>
     <t>16:00-19:00</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>19:00-23:00</t>
   </si>
   <si>
     <t>14:00-17:00</t>
-  </si>
-  <si>
-    <t>3*</t>
   </si>
   <si>
     <t>17:00-21:00</t>
@@ -144,15 +138,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -161,11 +158,20 @@
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -478,20 +484,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -499,341 +505,341 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2"/>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="2"/>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="5"/>
+      <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5" t="s">
+      <c r="N5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="6">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="5" t="s">
+      <c r="F9" s="2"/>
+      <c r="G9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N6" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="5" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="8">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="6">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="6">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="5" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="5" t="s">
+      <c r="L12" s="5"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="6">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="4"/>
       <c r="N13" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
skip slots that misses complete info of time interval or people needed
</commit_message>
<xml_diff>
--- a/schedule_template.xlsx
+++ b/schedule_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>SUN</t>
   </si>
@@ -61,10 +61,13 @@
     <t>10:00-13:00</t>
   </si>
   <si>
+    <t>dooo</t>
+  </si>
+  <si>
     <t>13:30-16:30</t>
   </si>
   <si>
-    <t>11:30-14:30</t>
+    <t>hello</t>
   </si>
   <si>
     <t>12:00-14:00</t>
@@ -622,7 +625,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="6" t="s">
@@ -642,11 +645,11 @@
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
@@ -654,11 +657,11 @@
       <c r="I6" s="4"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N6" s="5"/>
     </row>
@@ -688,23 +691,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
@@ -740,27 +743,27 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="4"/>
@@ -800,19 +803,19 @@
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="4"/>
@@ -836,7 +839,7 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="4"/>

</xml_diff>

<commit_message>
click me and report
</commit_message>
<xml_diff>
--- a/schedule_template.xlsx
+++ b/schedule_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>SUN</t>
   </si>
@@ -61,13 +61,10 @@
     <t>10:00-13:00</t>
   </si>
   <si>
-    <t>dooo</t>
-  </si>
-  <si>
     <t>13:30-16:30</t>
   </si>
   <si>
-    <t>hello</t>
+    <t>11:30-14:30</t>
   </si>
   <si>
     <t>12:00-14:00</t>
@@ -625,7 +622,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="6" t="s">
@@ -645,11 +642,11 @@
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
@@ -657,11 +654,11 @@
       <c r="I6" s="4"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N6" s="5"/>
     </row>
@@ -691,23 +688,23 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
@@ -743,27 +740,27 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="4"/>
@@ -803,19 +800,19 @@
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="4"/>
@@ -839,7 +836,7 @@
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="4"/>

</xml_diff>